<commit_message>
added a protocol to the main document
</commit_message>
<xml_diff>
--- a/bea-documentation/sprint-backlog/sprint-backlog.xlsx
+++ b/bea-documentation/sprint-backlog/sprint-backlog.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6168261-2793-43AD-ACC3-0DB1E1A6E81A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD86D9B9-78BC-4C31-BF20-6E54C9FF04BD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sprint plan" sheetId="8" r:id="rId1"/>
@@ -776,42 +776,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -858,6 +822,42 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1325,16 +1325,16 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>276224</xdr:colOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>223837</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
+      <xdr:colOff>428625</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1349,7 +1349,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11072812" y="276225"/>
+          <a:off x="10901362" y="266700"/>
           <a:ext cx="204788" cy="114300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1654,8 +1654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52C5C85A-82B4-4FC3-85DE-ADD80C9606CE}">
   <dimension ref="A1:AC22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1689,606 +1689,606 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29">
-      <c r="A1" s="34"/>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34"/>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
-      <c r="T1" s="37"/>
-      <c r="U1" s="37"/>
-      <c r="V1" s="37"/>
-      <c r="W1" s="37"/>
-      <c r="X1" s="37"/>
-      <c r="Y1" s="37"/>
-      <c r="Z1" s="37"/>
+      <c r="A1" s="22"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="25"/>
+      <c r="U1" s="25"/>
+      <c r="V1" s="25"/>
+      <c r="W1" s="25"/>
+      <c r="X1" s="25"/>
+      <c r="Y1" s="25"/>
+      <c r="Z1" s="25"/>
     </row>
     <row r="2" spans="1:29">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="34"/>
-      <c r="Q2" s="34"/>
-      <c r="R2" s="34"/>
-      <c r="S2" s="34"/>
-      <c r="T2" s="37"/>
-      <c r="U2" s="38"/>
-      <c r="V2" s="39"/>
-      <c r="W2" s="39"/>
-      <c r="X2" s="39"/>
-      <c r="Y2" s="39"/>
-      <c r="Z2" s="39"/>
-      <c r="AA2" s="39"/>
-      <c r="AB2" s="39"/>
-      <c r="AC2" s="40"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22"/>
+      <c r="S2" s="22"/>
+      <c r="T2" s="25"/>
+      <c r="U2" s="26"/>
+      <c r="V2" s="27"/>
+      <c r="W2" s="27"/>
+      <c r="X2" s="27"/>
+      <c r="Y2" s="27"/>
+      <c r="Z2" s="27"/>
+      <c r="AA2" s="27"/>
+      <c r="AB2" s="27"/>
+      <c r="AC2" s="28"/>
     </row>
     <row r="3" spans="1:29">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="34"/>
-      <c r="K3" s="34"/>
-      <c r="L3" s="34"/>
-      <c r="M3" s="34"/>
-      <c r="N3" s="34"/>
-      <c r="O3" s="34"/>
-      <c r="P3" s="34"/>
-      <c r="Q3" s="34"/>
-      <c r="R3" s="34"/>
-      <c r="S3" s="34"/>
-      <c r="T3" s="37"/>
-      <c r="U3" s="41"/>
-      <c r="V3" s="42"/>
-      <c r="W3" s="42"/>
-      <c r="X3" s="42"/>
-      <c r="Y3" s="42"/>
-      <c r="Z3" s="42"/>
-      <c r="AA3" s="42"/>
-      <c r="AB3" s="42"/>
-      <c r="AC3" s="43"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="22"/>
+      <c r="Q3" s="22"/>
+      <c r="R3" s="22"/>
+      <c r="S3" s="22"/>
+      <c r="T3" s="25"/>
+      <c r="U3" s="29"/>
+      <c r="V3" s="30"/>
+      <c r="W3" s="30"/>
+      <c r="X3" s="30"/>
+      <c r="Y3" s="30"/>
+      <c r="Z3" s="30"/>
+      <c r="AA3" s="30"/>
+      <c r="AB3" s="30"/>
+      <c r="AC3" s="31"/>
     </row>
     <row r="4" spans="1:29">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="34"/>
-      <c r="K4" s="34"/>
-      <c r="L4" s="34"/>
-      <c r="M4" s="34"/>
-      <c r="N4" s="34"/>
-      <c r="O4" s="34"/>
-      <c r="P4" s="34"/>
-      <c r="Q4" s="34"/>
-      <c r="R4" s="34"/>
-      <c r="S4" s="34"/>
-      <c r="T4" s="37"/>
-      <c r="U4" s="41"/>
-      <c r="V4" s="44">
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="22"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="22"/>
+      <c r="Q4" s="22"/>
+      <c r="R4" s="22"/>
+      <c r="S4" s="22"/>
+      <c r="T4" s="25"/>
+      <c r="U4" s="29"/>
+      <c r="V4" s="32">
         <v>43739</v>
       </c>
-      <c r="W4" s="42"/>
-      <c r="X4" s="42"/>
-      <c r="Y4" s="42"/>
-      <c r="Z4" s="42"/>
-      <c r="AA4" s="42"/>
-      <c r="AB4" s="42"/>
-      <c r="AC4" s="43"/>
+      <c r="W4" s="30"/>
+      <c r="X4" s="30"/>
+      <c r="Y4" s="30"/>
+      <c r="Z4" s="30"/>
+      <c r="AA4" s="30"/>
+      <c r="AB4" s="30"/>
+      <c r="AC4" s="31"/>
     </row>
     <row r="5" spans="1:29">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="34">
+      <c r="B5" s="22">
         <v>36</v>
       </c>
-      <c r="C5" s="34">
+      <c r="C5" s="22">
         <v>37</v>
       </c>
-      <c r="D5" s="34">
+      <c r="D5" s="22">
         <v>38</v>
       </c>
-      <c r="E5" s="34">
+      <c r="E5" s="22">
         <v>39</v>
       </c>
-      <c r="F5" s="34">
+      <c r="F5" s="22">
         <v>40</v>
       </c>
-      <c r="G5" s="34">
+      <c r="G5" s="22">
         <v>41</v>
       </c>
-      <c r="H5" s="34">
+      <c r="H5" s="22">
         <v>42</v>
       </c>
-      <c r="I5" s="34">
+      <c r="I5" s="22">
         <v>43</v>
       </c>
-      <c r="J5" s="34">
+      <c r="J5" s="22">
         <v>44</v>
       </c>
-      <c r="K5" s="34">
+      <c r="K5" s="22">
         <v>45</v>
       </c>
-      <c r="L5" s="34">
+      <c r="L5" s="22">
         <v>46</v>
       </c>
-      <c r="M5" s="34">
+      <c r="M5" s="22">
         <v>47</v>
       </c>
-      <c r="N5" s="34">
+      <c r="N5" s="22">
         <v>48</v>
       </c>
-      <c r="O5" s="34">
+      <c r="O5" s="22">
         <v>49</v>
       </c>
-      <c r="P5" s="34">
+      <c r="P5" s="22">
         <v>50</v>
       </c>
-      <c r="Q5" s="34">
+      <c r="Q5" s="22">
         <v>51</v>
       </c>
-      <c r="R5" s="34">
+      <c r="R5" s="22">
         <v>52</v>
       </c>
-      <c r="S5" s="34">
+      <c r="S5" s="22">
         <v>1</v>
       </c>
-      <c r="T5" s="37"/>
-      <c r="U5" s="45" t="s">
+      <c r="T5" s="25"/>
+      <c r="U5" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="V5" s="42" t="s">
+      <c r="V5" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="W5" s="42" t="s">
+      <c r="W5" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="X5" s="42" t="s">
+      <c r="X5" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="Y5" s="42" t="s">
+      <c r="Y5" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="Z5" s="42" t="s">
+      <c r="Z5" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="AA5" s="42" t="s">
+      <c r="AA5" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="AB5" s="42" t="s">
+      <c r="AB5" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="AC5" s="46" t="s">
+      <c r="AC5" s="34" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:29">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34">
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22">
         <v>1</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="22">
         <v>2</v>
       </c>
-      <c r="F6" s="34">
+      <c r="F6" s="22">
         <v>3</v>
       </c>
-      <c r="G6" s="34">
+      <c r="G6" s="22">
         <v>4</v>
       </c>
-      <c r="H6" s="34">
+      <c r="H6" s="22">
         <v>5</v>
       </c>
-      <c r="I6" s="34">
+      <c r="I6" s="22">
         <v>6</v>
       </c>
-      <c r="J6" s="34">
+      <c r="J6" s="22">
         <v>7</v>
       </c>
-      <c r="K6" s="34">
+      <c r="K6" s="22">
         <v>8</v>
       </c>
-      <c r="L6" s="34">
+      <c r="L6" s="22">
         <v>9</v>
       </c>
-      <c r="M6" s="34">
+      <c r="M6" s="22">
         <v>10</v>
       </c>
-      <c r="N6" s="34">
+      <c r="N6" s="22">
         <v>11</v>
       </c>
-      <c r="O6" s="34">
+      <c r="O6" s="22">
         <v>12</v>
       </c>
-      <c r="P6" s="34">
+      <c r="P6" s="22">
         <v>13</v>
       </c>
-      <c r="Q6" s="34">
+      <c r="Q6" s="22">
         <v>14</v>
       </c>
-      <c r="R6" s="35" t="s">
+      <c r="R6" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="S6" s="35" t="s">
+      <c r="S6" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="T6" s="37"/>
-      <c r="U6" s="45"/>
-      <c r="V6" s="42"/>
-      <c r="W6" s="42"/>
-      <c r="X6" s="47">
+      <c r="T6" s="25"/>
+      <c r="U6" s="33"/>
+      <c r="V6" s="30"/>
+      <c r="W6" s="30"/>
+      <c r="X6" s="35">
         <v>2</v>
       </c>
-      <c r="Y6" s="42"/>
-      <c r="Z6" s="42"/>
-      <c r="AA6" s="42"/>
-      <c r="AB6" s="42"/>
-      <c r="AC6" s="48"/>
+      <c r="Y6" s="30"/>
+      <c r="Z6" s="30"/>
+      <c r="AA6" s="30"/>
+      <c r="AB6" s="30"/>
+      <c r="AC6" s="36"/>
     </row>
     <row r="7" spans="1:29">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="35">
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="23">
         <v>1</v>
       </c>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="55">
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="43">
         <v>2</v>
       </c>
-      <c r="I7" s="55"/>
-      <c r="J7" s="55"/>
-      <c r="K7" s="56">
+      <c r="I7" s="43"/>
+      <c r="J7" s="43"/>
+      <c r="K7" s="44">
         <v>3</v>
       </c>
-      <c r="L7" s="56"/>
-      <c r="M7" s="56"/>
-      <c r="N7" s="57">
+      <c r="L7" s="44"/>
+      <c r="M7" s="44"/>
+      <c r="N7" s="45">
         <v>4</v>
       </c>
-      <c r="O7" s="57"/>
-      <c r="P7" s="57"/>
-      <c r="Q7" s="57"/>
-      <c r="R7" s="34"/>
-      <c r="S7" s="34"/>
-      <c r="T7" s="37"/>
-      <c r="U7" s="45"/>
-      <c r="V7" s="42"/>
-      <c r="W7" s="42"/>
-      <c r="X7" s="47">
+      <c r="O7" s="45"/>
+      <c r="P7" s="45"/>
+      <c r="Q7" s="45"/>
+      <c r="R7" s="22"/>
+      <c r="S7" s="22"/>
+      <c r="T7" s="25"/>
+      <c r="U7" s="33"/>
+      <c r="V7" s="30"/>
+      <c r="W7" s="30"/>
+      <c r="X7" s="35">
         <v>9</v>
       </c>
-      <c r="Y7" s="42"/>
-      <c r="Z7" s="42"/>
-      <c r="AA7" s="42"/>
-      <c r="AB7" s="42"/>
-      <c r="AC7" s="48"/>
+      <c r="Y7" s="30"/>
+      <c r="Z7" s="30"/>
+      <c r="AA7" s="30"/>
+      <c r="AB7" s="30"/>
+      <c r="AC7" s="36"/>
     </row>
     <row r="8" spans="1:29">
-      <c r="A8" s="34"/>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34" t="s">
+      <c r="A8" s="22"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
-      <c r="J8" s="34" t="s">
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="K8" s="34"/>
-      <c r="L8" s="34"/>
-      <c r="M8" s="34" t="s">
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="N8" s="34"/>
-      <c r="O8" s="34"/>
-      <c r="P8" s="34"/>
-      <c r="Q8" s="34" t="s">
+      <c r="N8" s="22"/>
+      <c r="O8" s="22"/>
+      <c r="P8" s="22"/>
+      <c r="Q8" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="R8" s="34"/>
-      <c r="S8" s="34"/>
-      <c r="T8" s="37"/>
-      <c r="U8" s="45"/>
-      <c r="V8" s="42"/>
-      <c r="W8" s="42"/>
-      <c r="X8" s="47">
+      <c r="R8" s="22"/>
+      <c r="S8" s="22"/>
+      <c r="T8" s="25"/>
+      <c r="U8" s="33"/>
+      <c r="V8" s="30"/>
+      <c r="W8" s="30"/>
+      <c r="X8" s="35">
         <v>16</v>
       </c>
-      <c r="Y8" s="42"/>
-      <c r="Z8" s="42"/>
-      <c r="AA8" s="42"/>
-      <c r="AB8" s="42"/>
-      <c r="AC8" s="48"/>
+      <c r="Y8" s="30"/>
+      <c r="Z8" s="30"/>
+      <c r="AA8" s="30"/>
+      <c r="AB8" s="30"/>
+      <c r="AC8" s="36"/>
     </row>
     <row r="9" spans="1:29">
-      <c r="A9" s="34"/>
-      <c r="B9" s="34"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34"/>
-      <c r="J9" s="34"/>
-      <c r="K9" s="34"/>
-      <c r="L9" s="34"/>
-      <c r="M9" s="34"/>
-      <c r="N9" s="34"/>
-      <c r="O9" s="34"/>
-      <c r="P9" s="34"/>
-      <c r="Q9" s="34"/>
-      <c r="R9" s="34"/>
-      <c r="S9" s="34"/>
-      <c r="T9" s="37"/>
-      <c r="U9" s="45"/>
-      <c r="V9" s="42"/>
-      <c r="W9" s="42"/>
-      <c r="X9" s="47">
+      <c r="A9" s="22"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22"/>
+      <c r="O9" s="22"/>
+      <c r="P9" s="22"/>
+      <c r="Q9" s="22"/>
+      <c r="R9" s="22"/>
+      <c r="S9" s="22"/>
+      <c r="T9" s="25"/>
+      <c r="U9" s="33"/>
+      <c r="V9" s="30"/>
+      <c r="W9" s="30"/>
+      <c r="X9" s="35">
         <v>23</v>
       </c>
-      <c r="Y9" s="42"/>
-      <c r="Z9" s="42"/>
-      <c r="AA9" s="42"/>
-      <c r="AB9" s="42"/>
-      <c r="AC9" s="48"/>
+      <c r="Y9" s="30"/>
+      <c r="Z9" s="30"/>
+      <c r="AA9" s="30"/>
+      <c r="AB9" s="30"/>
+      <c r="AC9" s="36"/>
     </row>
     <row r="10" spans="1:29">
-      <c r="A10" s="34"/>
-      <c r="B10" s="34"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="34"/>
-      <c r="K10" s="34"/>
-      <c r="L10" s="34"/>
-      <c r="M10" s="34"/>
-      <c r="N10" s="34"/>
-      <c r="O10" s="34"/>
-      <c r="P10" s="34"/>
-      <c r="Q10" s="34"/>
-      <c r="R10" s="34"/>
-      <c r="S10" s="34"/>
-      <c r="T10" s="37"/>
-      <c r="U10" s="45"/>
-      <c r="V10" s="42"/>
-      <c r="W10" s="42"/>
-      <c r="X10" s="47">
+      <c r="A10" s="22"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="22"/>
+      <c r="P10" s="22"/>
+      <c r="Q10" s="22"/>
+      <c r="R10" s="22"/>
+      <c r="S10" s="22"/>
+      <c r="T10" s="25"/>
+      <c r="U10" s="33"/>
+      <c r="V10" s="30"/>
+      <c r="W10" s="30"/>
+      <c r="X10" s="35">
         <v>30</v>
       </c>
-      <c r="Y10" s="42"/>
-      <c r="Z10" s="42"/>
-      <c r="AA10" s="42"/>
-      <c r="AB10" s="42"/>
-      <c r="AC10" s="48"/>
+      <c r="Y10" s="30"/>
+      <c r="Z10" s="30"/>
+      <c r="AA10" s="30"/>
+      <c r="AB10" s="30"/>
+      <c r="AC10" s="36"/>
     </row>
     <row r="11" spans="1:29">
-      <c r="A11" s="34"/>
-      <c r="B11" s="34"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
-      <c r="J11" s="34"/>
-      <c r="K11" s="34"/>
-      <c r="L11" s="34"/>
-      <c r="M11" s="34"/>
-      <c r="N11" s="34"/>
-      <c r="O11" s="34"/>
-      <c r="P11" s="34"/>
-      <c r="Q11" s="34"/>
-      <c r="R11" s="34"/>
-      <c r="S11" s="34"/>
-      <c r="T11" s="37"/>
-      <c r="U11" s="45"/>
-      <c r="V11" s="44">
+      <c r="A11" s="22"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="22"/>
+      <c r="M11" s="22"/>
+      <c r="N11" s="22"/>
+      <c r="O11" s="22"/>
+      <c r="P11" s="22"/>
+      <c r="Q11" s="22"/>
+      <c r="R11" s="22"/>
+      <c r="S11" s="22"/>
+      <c r="T11" s="25"/>
+      <c r="U11" s="33"/>
+      <c r="V11" s="32">
         <v>43770</v>
       </c>
-      <c r="W11" s="42"/>
-      <c r="X11" s="47"/>
-      <c r="Y11" s="42"/>
-      <c r="Z11" s="42"/>
-      <c r="AA11" s="42"/>
-      <c r="AB11" s="42"/>
-      <c r="AC11" s="48"/>
+      <c r="W11" s="30"/>
+      <c r="X11" s="35"/>
+      <c r="Y11" s="30"/>
+      <c r="Z11" s="30"/>
+      <c r="AA11" s="30"/>
+      <c r="AB11" s="30"/>
+      <c r="AC11" s="36"/>
     </row>
     <row r="12" spans="1:29">
-      <c r="U12" s="45"/>
-      <c r="V12" s="42"/>
-      <c r="W12" s="42"/>
-      <c r="X12" s="47">
+      <c r="U12" s="33"/>
+      <c r="V12" s="30"/>
+      <c r="W12" s="30"/>
+      <c r="X12" s="35">
         <v>6</v>
       </c>
-      <c r="Y12" s="42"/>
-      <c r="Z12" s="42"/>
-      <c r="AA12" s="42"/>
-      <c r="AB12" s="42"/>
-      <c r="AC12" s="48"/>
+      <c r="Y12" s="30"/>
+      <c r="Z12" s="30"/>
+      <c r="AA12" s="30"/>
+      <c r="AB12" s="30"/>
+      <c r="AC12" s="36"/>
     </row>
     <row r="13" spans="1:29">
-      <c r="U13" s="45"/>
-      <c r="V13" s="42"/>
-      <c r="W13" s="42"/>
-      <c r="X13" s="47">
+      <c r="U13" s="33"/>
+      <c r="V13" s="30"/>
+      <c r="W13" s="30"/>
+      <c r="X13" s="35">
         <v>13</v>
       </c>
-      <c r="Y13" s="42"/>
-      <c r="Z13" s="42"/>
-      <c r="AA13" s="42"/>
-      <c r="AB13" s="42"/>
-      <c r="AC13" s="48"/>
+      <c r="Y13" s="30"/>
+      <c r="Z13" s="30"/>
+      <c r="AA13" s="30"/>
+      <c r="AB13" s="30"/>
+      <c r="AC13" s="36"/>
     </row>
     <row r="14" spans="1:29">
-      <c r="D14" s="36"/>
-      <c r="U14" s="45"/>
-      <c r="V14" s="42"/>
-      <c r="W14" s="42"/>
-      <c r="X14" s="47">
+      <c r="D14" s="24"/>
+      <c r="U14" s="33"/>
+      <c r="V14" s="30"/>
+      <c r="W14" s="30"/>
+      <c r="X14" s="35">
         <v>20</v>
       </c>
-      <c r="Y14" s="42"/>
-      <c r="Z14" s="42"/>
-      <c r="AA14" s="42"/>
-      <c r="AB14" s="42"/>
-      <c r="AC14" s="48"/>
+      <c r="Y14" s="30"/>
+      <c r="Z14" s="30"/>
+      <c r="AA14" s="30"/>
+      <c r="AB14" s="30"/>
+      <c r="AC14" s="36"/>
     </row>
     <row r="15" spans="1:29">
-      <c r="D15" s="36"/>
-      <c r="U15" s="45"/>
-      <c r="V15" s="42"/>
-      <c r="W15" s="42"/>
-      <c r="X15" s="47">
+      <c r="D15" s="24"/>
+      <c r="U15" s="33"/>
+      <c r="V15" s="30"/>
+      <c r="W15" s="30"/>
+      <c r="X15" s="35">
         <v>27</v>
       </c>
-      <c r="Y15" s="42"/>
-      <c r="Z15" s="42"/>
-      <c r="AA15" s="42"/>
-      <c r="AB15" s="42"/>
-      <c r="AC15" s="48"/>
+      <c r="Y15" s="30"/>
+      <c r="Z15" s="30"/>
+      <c r="AA15" s="30"/>
+      <c r="AB15" s="30"/>
+      <c r="AC15" s="36"/>
     </row>
     <row r="16" spans="1:29">
-      <c r="D16" s="36"/>
-      <c r="U16" s="45"/>
-      <c r="V16" s="44">
+      <c r="D16" s="24"/>
+      <c r="U16" s="33"/>
+      <c r="V16" s="32">
         <v>43800</v>
       </c>
-      <c r="W16" s="42"/>
-      <c r="X16" s="47"/>
-      <c r="Y16" s="42"/>
-      <c r="Z16" s="42"/>
-      <c r="AA16" s="42"/>
-      <c r="AB16" s="42"/>
-      <c r="AC16" s="48"/>
+      <c r="W16" s="30"/>
+      <c r="X16" s="35"/>
+      <c r="Y16" s="30"/>
+      <c r="Z16" s="30"/>
+      <c r="AA16" s="30"/>
+      <c r="AB16" s="30"/>
+      <c r="AC16" s="36"/>
     </row>
     <row r="17" spans="4:29">
-      <c r="D17" s="36"/>
-      <c r="U17" s="45"/>
-      <c r="V17" s="42"/>
-      <c r="W17" s="42"/>
-      <c r="X17" s="47">
+      <c r="D17" s="24"/>
+      <c r="U17" s="33"/>
+      <c r="V17" s="30"/>
+      <c r="W17" s="30"/>
+      <c r="X17" s="35">
         <v>4</v>
       </c>
-      <c r="Y17" s="42"/>
-      <c r="Z17" s="42"/>
-      <c r="AA17" s="42"/>
-      <c r="AB17" s="42"/>
-      <c r="AC17" s="48"/>
+      <c r="Y17" s="30"/>
+      <c r="Z17" s="30"/>
+      <c r="AA17" s="30"/>
+      <c r="AB17" s="30"/>
+      <c r="AC17" s="36"/>
     </row>
     <row r="18" spans="4:29">
-      <c r="D18" s="36"/>
-      <c r="U18" s="45"/>
-      <c r="V18" s="42"/>
-      <c r="W18" s="42"/>
-      <c r="X18" s="47">
+      <c r="D18" s="24"/>
+      <c r="U18" s="33"/>
+      <c r="V18" s="30"/>
+      <c r="W18" s="30"/>
+      <c r="X18" s="35">
         <v>11</v>
       </c>
-      <c r="Y18" s="42"/>
-      <c r="Z18" s="42"/>
-      <c r="AA18" s="42"/>
-      <c r="AB18" s="42"/>
-      <c r="AC18" s="48"/>
+      <c r="Y18" s="30"/>
+      <c r="Z18" s="30"/>
+      <c r="AA18" s="30"/>
+      <c r="AB18" s="30"/>
+      <c r="AC18" s="36"/>
     </row>
     <row r="19" spans="4:29">
-      <c r="U19" s="49"/>
-      <c r="V19" s="50"/>
-      <c r="W19" s="50"/>
-      <c r="X19" s="51">
+      <c r="U19" s="37"/>
+      <c r="V19" s="38"/>
+      <c r="W19" s="38"/>
+      <c r="X19" s="39">
         <v>18</v>
       </c>
-      <c r="Y19" s="50"/>
-      <c r="Z19" s="50"/>
-      <c r="AA19" s="50"/>
-      <c r="AB19" s="50"/>
-      <c r="AC19" s="52"/>
+      <c r="Y19" s="38"/>
+      <c r="Z19" s="38"/>
+      <c r="AA19" s="38"/>
+      <c r="AB19" s="38"/>
+      <c r="AC19" s="40"/>
     </row>
     <row r="20" spans="4:29">
-      <c r="V20" s="37"/>
-      <c r="W20" s="37"/>
-      <c r="X20" s="37"/>
-      <c r="Y20" s="37"/>
-      <c r="Z20" s="37"/>
-      <c r="AA20" s="37"/>
-      <c r="AB20" s="37"/>
+      <c r="V20" s="25"/>
+      <c r="W20" s="25"/>
+      <c r="X20" s="25"/>
+      <c r="Y20" s="25"/>
+      <c r="Z20" s="25"/>
+      <c r="AA20" s="25"/>
+      <c r="AB20" s="25"/>
     </row>
     <row r="21" spans="4:29">
-      <c r="V21" s="37"/>
-      <c r="W21" s="37"/>
-      <c r="X21" s="37"/>
-      <c r="Y21" s="37"/>
-      <c r="Z21" s="37"/>
-      <c r="AA21" s="37"/>
-      <c r="AB21" s="37"/>
+      <c r="V21" s="25"/>
+      <c r="W21" s="25"/>
+      <c r="X21" s="25"/>
+      <c r="Y21" s="25"/>
+      <c r="Z21" s="25"/>
+      <c r="AA21" s="25"/>
+      <c r="AB21" s="25"/>
     </row>
     <row r="22" spans="4:29">
-      <c r="V22" s="53" t="s">
+      <c r="V22" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="W22" s="53"/>
-      <c r="X22" s="53"/>
-      <c r="Y22" s="53"/>
-      <c r="Z22" s="37"/>
-      <c r="AA22" s="37"/>
-      <c r="AB22" s="37"/>
+      <c r="W22" s="41"/>
+      <c r="X22" s="41"/>
+      <c r="Y22" s="41"/>
+      <c r="Z22" s="25"/>
+      <c r="AA22" s="25"/>
+      <c r="AB22" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2300,8 +2300,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2312,20 +2312,20 @@
     <col min="4" max="4" width="5.9296875" customWidth="1"/>
     <col min="5" max="5" width="4.6640625" customWidth="1"/>
     <col min="6" max="6" width="6.9296875" customWidth="1"/>
-    <col min="7" max="7" width="8.3984375" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" customWidth="1"/>
     <col min="8" max="8" width="4" customWidth="1"/>
     <col min="9" max="9" width="36.33203125" customWidth="1"/>
     <col min="10" max="10" width="30.73046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="32.25" customHeight="1" thickBot="1">
-      <c r="C1" s="60" t="s">
+      <c r="C1" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="F1" s="54" t="s">
+      <c r="F1" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="G1" s="54"/>
+      <c r="G1" s="42"/>
     </row>
     <row r="2" spans="1:10" ht="58.5" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -2350,10 +2350,10 @@
         <v>2</v>
       </c>
       <c r="H2" s="3"/>
-      <c r="I2" s="63" t="s">
+      <c r="I2" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="J2" s="64" t="s">
+      <c r="J2" s="52" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2376,10 +2376,10 @@
         <v>19</v>
       </c>
       <c r="H3" s="6"/>
-      <c r="I3" s="65" t="s">
+      <c r="I3" s="53" t="s">
         <v>55</v>
       </c>
-      <c r="J3" s="66" t="s">
+      <c r="J3" s="54" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2402,10 +2402,10 @@
         <v>19</v>
       </c>
       <c r="H4" s="19"/>
-      <c r="I4" s="67" t="s">
+      <c r="I4" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="J4" s="68" t="s">
+      <c r="J4" s="56" t="s">
         <v>60</v>
       </c>
     </row>
@@ -2428,10 +2428,10 @@
         <v>19</v>
       </c>
       <c r="H5" s="20"/>
-      <c r="I5" s="65" t="s">
+      <c r="I5" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="66" t="s">
+      <c r="J5" s="54" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2454,10 +2454,10 @@
         <v>19</v>
       </c>
       <c r="H6" s="21"/>
-      <c r="I6" s="67" t="s">
+      <c r="I6" s="55" t="s">
         <v>57</v>
       </c>
-      <c r="J6" s="68" t="s">
+      <c r="J6" s="56" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2481,11 +2481,11 @@
       <c r="G7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="28"/>
-      <c r="I7" s="65" t="s">
+      <c r="H7" s="60"/>
+      <c r="I7" s="53" t="s">
         <v>58</v>
       </c>
-      <c r="J7" s="66" t="s">
+      <c r="J7" s="54" t="s">
         <v>63</v>
       </c>
     </row>
@@ -2507,11 +2507,11 @@
       <c r="G8" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="H8" s="29"/>
-      <c r="I8" s="67" t="s">
+      <c r="H8" s="61"/>
+      <c r="I8" s="55" t="s">
         <v>102</v>
       </c>
-      <c r="J8" s="68" t="s">
+      <c r="J8" s="56" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2533,11 +2533,11 @@
       <c r="G9" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="28"/>
-      <c r="I9" s="65" t="s">
+      <c r="H9" s="60"/>
+      <c r="I9" s="53" t="s">
         <v>103</v>
       </c>
-      <c r="J9" s="66" t="s">
+      <c r="J9" s="54" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2559,9 +2559,9 @@
       <c r="G10" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="H10" s="29"/>
-      <c r="I10" s="67"/>
-      <c r="J10" s="68" t="s">
+      <c r="H10" s="61"/>
+      <c r="I10" s="55"/>
+      <c r="J10" s="56" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2579,83 +2579,79 @@
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
       <c r="G11" s="17"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="65"/>
-      <c r="J11" s="66"/>
+      <c r="H11" s="62"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="54"/>
     </row>
     <row r="12" spans="1:10" ht="14.65" thickBot="1">
-      <c r="A12" s="24">
+      <c r="A12" s="66">
         <v>10</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="22" t="s">
+      <c r="D12" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="28" t="s">
+      <c r="E12" s="64"/>
+      <c r="F12" s="64"/>
+      <c r="G12" s="60" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="63"/>
+      <c r="I12" s="55"/>
+      <c r="J12" s="56"/>
+    </row>
+    <row r="13" spans="1:10" ht="14.65" thickBot="1">
+      <c r="A13" s="67"/>
+      <c r="B13" s="63"/>
+      <c r="C13" s="63"/>
+      <c r="D13" s="63"/>
+      <c r="E13" s="65"/>
+      <c r="F13" s="65"/>
+      <c r="G13" s="61"/>
+      <c r="I13" s="53"/>
+      <c r="J13" s="54"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="66">
+        <v>11</v>
+      </c>
+      <c r="B14" s="60" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="60" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="68" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="64"/>
+      <c r="F14" s="64"/>
+      <c r="G14" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="H12" s="23"/>
-      <c r="I12" s="67"/>
-      <c r="J12" s="68"/>
-    </row>
-    <row r="13" spans="1:10" ht="14.65" thickBot="1">
-      <c r="A13" s="25"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="29"/>
-      <c r="I13" s="65"/>
-      <c r="J13" s="66"/>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="24">
-        <v>11</v>
-      </c>
-      <c r="B14" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="I14" s="61"/>
-      <c r="J14" s="62"/>
+      <c r="I14" s="49"/>
+      <c r="J14" s="50"/>
     </row>
     <row r="15" spans="1:10" ht="14.65" thickBot="1">
-      <c r="A15" s="25"/>
-      <c r="B15" s="29"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="29"/>
+      <c r="A15" s="67"/>
+      <c r="B15" s="61"/>
+      <c r="C15" s="61"/>
+      <c r="D15" s="69"/>
+      <c r="E15" s="65"/>
+      <c r="F15" s="65"/>
+      <c r="G15" s="61"/>
     </row>
     <row r="18" spans="3:3" ht="23.25" customHeight="1"/>
     <row r="30" spans="3:3">
-      <c r="C30" s="59"/>
+      <c r="C30" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="F12:F13"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="C14:C15"/>
@@ -2669,6 +2665,10 @@
     <mergeCell ref="H9:H10"/>
     <mergeCell ref="H11:H12"/>
     <mergeCell ref="G12:G13"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="F12:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2693,13 +2693,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="34.5" customHeight="1" thickBot="1">
-      <c r="C1" s="59" t="s">
+      <c r="C1" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="F1" s="54" t="s">
+      <c r="F1" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="G1" s="54"/>
+      <c r="G1" s="42"/>
     </row>
     <row r="2" spans="1:10" ht="23.65" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -2724,10 +2724,10 @@
         <v>2</v>
       </c>
       <c r="H2" s="3"/>
-      <c r="I2" s="58" t="s">
+      <c r="I2" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="J2" s="69" t="s">
+      <c r="J2" s="57" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2813,7 +2813,7 @@
       <c r="D7" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="28"/>
+      <c r="H7" s="60"/>
       <c r="J7" t="s">
         <v>86</v>
       </c>
@@ -2831,42 +2831,42 @@
       <c r="D8" t="s">
         <v>29</v>
       </c>
-      <c r="H8" s="29"/>
+      <c r="H8" s="61"/>
       <c r="J8" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="H9" s="28"/>
+      <c r="H9" s="60"/>
     </row>
     <row r="10" spans="1:10" ht="14.65" thickBot="1">
-      <c r="H10" s="29"/>
+      <c r="H10" s="61"/>
       <c r="J10" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="24"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
+      <c r="A11" s="66"/>
+      <c r="B11" s="62"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="62"/>
+      <c r="H11" s="62"/>
       <c r="J11" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="14.65" thickBot="1">
-      <c r="A12" s="25"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
+      <c r="A12" s="67"/>
+      <c r="B12" s="63"/>
+      <c r="C12" s="63"/>
+      <c r="D12" s="63"/>
+      <c r="E12" s="71"/>
+      <c r="F12" s="71"/>
+      <c r="G12" s="63"/>
+      <c r="H12" s="63"/>
       <c r="J12" t="s">
         <v>96</v>
       </c>
@@ -2877,27 +2877,27 @@
       </c>
     </row>
     <row r="15" spans="1:10">
-      <c r="J15" s="70" t="s">
+      <c r="J15" s="58" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:10">
-      <c r="J16" s="71" t="s">
+      <c r="J16" s="59" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="17" spans="10:10">
-      <c r="J17" s="71" t="s">
+      <c r="J17" s="59" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="18" spans="10:10">
-      <c r="J18" s="71" t="s">
+      <c r="J18" s="59" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="19" spans="10:10">
-      <c r="J19" s="71" t="s">
+      <c r="J19" s="59" t="s">
         <v>95</v>
       </c>
     </row>
@@ -2936,10 +2936,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="32.25" customHeight="1" thickBot="1">
-      <c r="F1" s="54" t="s">
+      <c r="F1" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="G1" s="54"/>
+      <c r="G1" s="42"/>
     </row>
     <row r="2" spans="1:10" ht="23.65" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -3021,64 +3021,64 @@
       <c r="H7" s="17"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="24"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
+      <c r="A8" s="66"/>
+      <c r="B8" s="60"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="60"/>
+      <c r="H8" s="60"/>
     </row>
     <row r="9" spans="1:10" ht="14.65" thickBot="1">
-      <c r="A9" s="25"/>
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="29"/>
+      <c r="A9" s="67"/>
+      <c r="B9" s="61"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="69"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="65"/>
+      <c r="G9" s="61"/>
+      <c r="H9" s="61"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="24"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
+      <c r="A10" s="66"/>
+      <c r="B10" s="60"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="64"/>
+      <c r="F10" s="64"/>
+      <c r="G10" s="60"/>
+      <c r="H10" s="60"/>
     </row>
     <row r="11" spans="1:10" ht="14.65" thickBot="1">
-      <c r="A11" s="25"/>
-      <c r="B11" s="29"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="29"/>
+      <c r="A11" s="67"/>
+      <c r="B11" s="61"/>
+      <c r="C11" s="61"/>
+      <c r="D11" s="61"/>
+      <c r="E11" s="65"/>
+      <c r="F11" s="65"/>
+      <c r="G11" s="61"/>
+      <c r="H11" s="61"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="24"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
+      <c r="A12" s="66"/>
+      <c r="B12" s="62"/>
+      <c r="C12" s="62"/>
+      <c r="D12" s="62"/>
+      <c r="E12" s="70"/>
+      <c r="F12" s="70"/>
+      <c r="G12" s="62"/>
+      <c r="H12" s="62"/>
     </row>
     <row r="13" spans="1:10" ht="14.65" thickBot="1">
-      <c r="A13" s="25"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
+      <c r="A13" s="67"/>
+      <c r="B13" s="63"/>
+      <c r="C13" s="63"/>
+      <c r="D13" s="63"/>
+      <c r="E13" s="71"/>
+      <c r="F13" s="71"/>
+      <c r="G13" s="63"/>
+      <c r="H13" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="24">
@@ -3129,10 +3129,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="39" customHeight="1" thickBot="1">
-      <c r="F1" s="54" t="s">
+      <c r="F1" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="G1" s="54"/>
+      <c r="G1" s="42"/>
       <c r="H1" t="s">
         <v>82</v>
       </c>
@@ -3217,64 +3217,64 @@
       <c r="H7" s="17"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="24"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
+      <c r="A8" s="66"/>
+      <c r="B8" s="60"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="60"/>
+      <c r="H8" s="60"/>
     </row>
     <row r="9" spans="1:10" ht="14.65" thickBot="1">
-      <c r="A9" s="25"/>
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="29"/>
+      <c r="A9" s="67"/>
+      <c r="B9" s="61"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="69"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="65"/>
+      <c r="G9" s="61"/>
+      <c r="H9" s="61"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="24"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
+      <c r="A10" s="66"/>
+      <c r="B10" s="60"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="64"/>
+      <c r="F10" s="64"/>
+      <c r="G10" s="60"/>
+      <c r="H10" s="60"/>
     </row>
     <row r="11" spans="1:10" ht="14.65" thickBot="1">
-      <c r="A11" s="25"/>
-      <c r="B11" s="29"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="29"/>
+      <c r="A11" s="67"/>
+      <c r="B11" s="61"/>
+      <c r="C11" s="61"/>
+      <c r="D11" s="61"/>
+      <c r="E11" s="65"/>
+      <c r="F11" s="65"/>
+      <c r="G11" s="61"/>
+      <c r="H11" s="61"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="24"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
+      <c r="A12" s="66"/>
+      <c r="B12" s="62"/>
+      <c r="C12" s="62"/>
+      <c r="D12" s="62"/>
+      <c r="E12" s="70"/>
+      <c r="F12" s="70"/>
+      <c r="G12" s="62"/>
+      <c r="H12" s="62"/>
     </row>
     <row r="13" spans="1:10" ht="14.65" thickBot="1">
-      <c r="A13" s="25"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
+      <c r="A13" s="67"/>
+      <c r="B13" s="63"/>
+      <c r="C13" s="63"/>
+      <c r="D13" s="63"/>
+      <c r="E13" s="71"/>
+      <c r="F13" s="71"/>
+      <c r="G13" s="63"/>
+      <c r="H13" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="24">
@@ -3312,7 +3312,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3405,64 +3405,64 @@
       <c r="H7" s="17"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="24"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
+      <c r="A8" s="66"/>
+      <c r="B8" s="60"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="60"/>
+      <c r="H8" s="60"/>
     </row>
     <row r="9" spans="1:10" ht="14.65" thickBot="1">
-      <c r="A9" s="25"/>
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="29"/>
+      <c r="A9" s="67"/>
+      <c r="B9" s="61"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="69"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="65"/>
+      <c r="G9" s="61"/>
+      <c r="H9" s="61"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="24"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
+      <c r="A10" s="66"/>
+      <c r="B10" s="60"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="64"/>
+      <c r="F10" s="64"/>
+      <c r="G10" s="60"/>
+      <c r="H10" s="60"/>
     </row>
     <row r="11" spans="1:10" ht="14.65" thickBot="1">
-      <c r="A11" s="25"/>
-      <c r="B11" s="29"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="29"/>
+      <c r="A11" s="67"/>
+      <c r="B11" s="61"/>
+      <c r="C11" s="61"/>
+      <c r="D11" s="61"/>
+      <c r="E11" s="65"/>
+      <c r="F11" s="65"/>
+      <c r="G11" s="61"/>
+      <c r="H11" s="61"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="24"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
+      <c r="A12" s="66"/>
+      <c r="B12" s="62"/>
+      <c r="C12" s="62"/>
+      <c r="D12" s="62"/>
+      <c r="E12" s="70"/>
+      <c r="F12" s="70"/>
+      <c r="G12" s="62"/>
+      <c r="H12" s="62"/>
     </row>
     <row r="13" spans="1:10" ht="14.65" thickBot="1">
-      <c r="A13" s="25"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
+      <c r="A13" s="67"/>
+      <c r="B13" s="63"/>
+      <c r="C13" s="63"/>
+      <c r="D13" s="63"/>
+      <c r="E13" s="71"/>
+      <c r="F13" s="71"/>
+      <c r="G13" s="63"/>
+      <c r="H13" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="24">

</xml_diff>

<commit_message>
added product backlog to the bea-report
</commit_message>
<xml_diff>
--- a/bea-documentation/sprint-backlog/sprint-backlog.xlsx
+++ b/bea-documentation/sprint-backlog/sprint-backlog.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD86D9B9-78BC-4C31-BF20-6E54C9FF04BD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6233DACC-E7C1-423A-B215-FDCDED8FB2AC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="104">
   <si>
     <t>Estimated Effort</t>
   </si>
@@ -79,9 +79,6 @@
     <t>Sprint Backlog. Make a document with sprint planning. Divide work in 14 weeks .</t>
   </si>
   <si>
-    <t xml:space="preserve">Start a project. Start firsts classes </t>
-  </si>
-  <si>
     <t>Important</t>
   </si>
   <si>
@@ -344,6 +341,9 @@
   </si>
   <si>
     <t xml:space="preserve">   split PB items into tasks</t>
+  </si>
+  <si>
+    <t>Start a project. Start firsts classes for login function</t>
   </si>
 </sst>
 </file>
@@ -822,16 +822,22 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -840,16 +846,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1655,7 +1655,7 @@
   <dimension ref="A1:AC22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="X9" sqref="X9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1749,7 +1749,7 @@
     </row>
     <row r="3" spans="1:29">
       <c r="A3" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" s="22"/>
       <c r="C3" s="22"/>
@@ -1782,7 +1782,7 @@
     </row>
     <row r="4" spans="1:29">
       <c r="A4" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" s="22"/>
       <c r="C4" s="22"/>
@@ -1817,7 +1817,7 @@
     </row>
     <row r="5" spans="1:29">
       <c r="A5" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" s="22">
         <v>36</v>
@@ -1875,36 +1875,36 @@
       </c>
       <c r="T5" s="25"/>
       <c r="U5" s="33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="V5" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="W5" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="W5" s="30" t="s">
+      <c r="X5" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y5" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="X5" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y5" s="30" t="s">
+      <c r="Z5" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="Z5" s="30" t="s">
+      <c r="AA5" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="AA5" s="30" t="s">
+      <c r="AB5" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="AB5" s="30" t="s">
+      <c r="AC5" s="34" t="s">
         <v>44</v>
-      </c>
-      <c r="AC5" s="34" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:29">
       <c r="A6" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" s="22"/>
       <c r="C6" s="22"/>
@@ -1951,10 +1951,10 @@
         <v>14</v>
       </c>
       <c r="R6" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="S6" s="23" t="s">
         <v>47</v>
-      </c>
-      <c r="S6" s="23" t="s">
-        <v>48</v>
       </c>
       <c r="T6" s="25"/>
       <c r="U6" s="33"/>
@@ -1971,7 +1971,7 @@
     </row>
     <row r="7" spans="1:29">
       <c r="A7" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7" s="22"/>
       <c r="C7" s="22"/>
@@ -2020,23 +2020,23 @@
       <c r="E8" s="22"/>
       <c r="F8" s="22"/>
       <c r="G8" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H8" s="22"/>
       <c r="I8" s="22"/>
       <c r="J8" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K8" s="22"/>
       <c r="L8" s="22"/>
       <c r="M8" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N8" s="22"/>
       <c r="O8" s="22"/>
       <c r="P8" s="22"/>
       <c r="Q8" s="22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="R8" s="22"/>
       <c r="S8" s="22"/>
@@ -2281,7 +2281,7 @@
     </row>
     <row r="22" spans="4:29">
       <c r="V22" s="41" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="W22" s="41"/>
       <c r="X22" s="41"/>
@@ -2301,7 +2301,7 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2320,10 +2320,10 @@
   <sheetData>
     <row r="1" spans="1:10" ht="32.25" customHeight="1" thickBot="1">
       <c r="C1" s="48" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F1" s="42" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G1" s="42"/>
     </row>
@@ -2351,10 +2351,10 @@
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="51" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J2" s="52" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="14.65" thickBot="1">
@@ -2362,10 +2362,10 @@
         <v>0</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>10</v>
@@ -2373,14 +2373,14 @@
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
       <c r="G3" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H3" s="6"/>
       <c r="I3" s="53" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J3" s="54" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="23.25">
@@ -2388,10 +2388,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>10</v>
@@ -2399,14 +2399,14 @@
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
       <c r="G4" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H4" s="19"/>
       <c r="I4" s="55" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J4" s="56" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="14.65" thickBot="1">
@@ -2414,10 +2414,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>10</v>
@@ -2425,14 +2425,14 @@
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
       <c r="G5" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H5" s="20"/>
       <c r="I5" s="53" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J5" s="54" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="14.65" thickBot="1">
@@ -2440,10 +2440,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>10</v>
@@ -2451,14 +2451,14 @@
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
       <c r="G6" s="16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H6" s="21"/>
       <c r="I6" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J6" s="56" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="14.65" thickBot="1">
@@ -2476,17 +2476,17 @@
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" s="60"/>
+        <v>18</v>
+      </c>
+      <c r="H7" s="62"/>
       <c r="I7" s="53" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J7" s="54" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="14.65" thickBot="1">
@@ -2497,7 +2497,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>10</v>
@@ -2505,14 +2505,14 @@
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
       <c r="G8" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="H8" s="61"/>
+        <v>30</v>
+      </c>
+      <c r="H8" s="63"/>
       <c r="I8" s="55" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J8" s="56" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="14.65" thickBot="1">
@@ -2531,14 +2531,14 @@
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
       <c r="G9" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="H9" s="60"/>
+        <v>30</v>
+      </c>
+      <c r="H9" s="62"/>
       <c r="I9" s="53" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J9" s="54" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="23.65" thickBot="1">
@@ -2557,12 +2557,12 @@
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
       <c r="G10" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="H10" s="61"/>
+        <v>100</v>
+      </c>
+      <c r="H10" s="63"/>
       <c r="I10" s="55"/>
       <c r="J10" s="56" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="23.65" thickBot="1">
@@ -2570,81 +2570,81 @@
         <v>9</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
       <c r="G11" s="17"/>
-      <c r="H11" s="62"/>
+      <c r="H11" s="68"/>
       <c r="I11" s="53"/>
       <c r="J11" s="54"/>
     </row>
     <row r="12" spans="1:10" ht="14.65" thickBot="1">
-      <c r="A12" s="66">
+      <c r="A12" s="60">
         <v>10</v>
       </c>
-      <c r="B12" s="62" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="62" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="62" t="s">
+      <c r="B12" s="68" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="68" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="64"/>
-      <c r="F12" s="64"/>
-      <c r="G12" s="60" t="s">
-        <v>19</v>
-      </c>
-      <c r="H12" s="63"/>
+      <c r="E12" s="66"/>
+      <c r="F12" s="66"/>
+      <c r="G12" s="62" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" s="69"/>
       <c r="I12" s="55"/>
       <c r="J12" s="56"/>
     </row>
     <row r="13" spans="1:10" ht="14.65" thickBot="1">
-      <c r="A13" s="67"/>
-      <c r="B13" s="63"/>
-      <c r="C13" s="63"/>
-      <c r="D13" s="63"/>
-      <c r="E13" s="65"/>
-      <c r="F13" s="65"/>
-      <c r="G13" s="61"/>
+      <c r="A13" s="61"/>
+      <c r="B13" s="69"/>
+      <c r="C13" s="69"/>
+      <c r="D13" s="69"/>
+      <c r="E13" s="67"/>
+      <c r="F13" s="67"/>
+      <c r="G13" s="63"/>
       <c r="I13" s="53"/>
       <c r="J13" s="54"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="66">
+      <c r="A14" s="60">
         <v>11</v>
       </c>
-      <c r="B14" s="60" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="60" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="68" t="s">
-        <v>29</v>
-      </c>
-      <c r="E14" s="64"/>
-      <c r="F14" s="64"/>
-      <c r="G14" s="60" t="s">
-        <v>31</v>
+      <c r="B14" s="62" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="62" t="s">
+        <v>103</v>
+      </c>
+      <c r="D14" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="66"/>
+      <c r="F14" s="66"/>
+      <c r="G14" s="62" t="s">
+        <v>30</v>
       </c>
       <c r="I14" s="49"/>
       <c r="J14" s="50"/>
     </row>
     <row r="15" spans="1:10" ht="14.65" thickBot="1">
-      <c r="A15" s="67"/>
-      <c r="B15" s="61"/>
-      <c r="C15" s="61"/>
-      <c r="D15" s="69"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="65"/>
-      <c r="G15" s="61"/>
+      <c r="A15" s="61"/>
+      <c r="B15" s="63"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="67"/>
+      <c r="F15" s="67"/>
+      <c r="G15" s="63"/>
     </row>
     <row r="18" spans="3:3" ht="23.25" customHeight="1"/>
     <row r="30" spans="3:3">
@@ -2652,6 +2652,14 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="F12:F13"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="C14:C15"/>
@@ -2661,14 +2669,6 @@
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="F12:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2679,7 +2679,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2694,10 +2694,10 @@
   <sheetData>
     <row r="1" spans="1:10" ht="34.5" customHeight="1" thickBot="1">
       <c r="C1" s="47" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F1" s="42" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G1" s="42"/>
     </row>
@@ -2725,10 +2725,10 @@
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="46" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J2" s="57" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="26.65" customHeight="1">
@@ -2736,17 +2736,17 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
       </c>
       <c r="H3" s="10"/>
       <c r="J3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="20.25" customHeight="1" thickBot="1">
@@ -2754,17 +2754,17 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
       </c>
       <c r="H4" s="13"/>
       <c r="J4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="18" customHeight="1">
@@ -2772,17 +2772,17 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
       </c>
       <c r="H5" s="16"/>
       <c r="J5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="18.75" customHeight="1" thickBot="1">
@@ -2790,13 +2790,16 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" t="s">
         <v>73</v>
-      </c>
-      <c r="C6" t="s">
-        <v>74</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
+      </c>
+      <c r="G6" t="s">
+        <v>18</v>
       </c>
       <c r="H6" s="17"/>
     </row>
@@ -2805,17 +2808,17 @@
         <v>16</v>
       </c>
       <c r="B7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" t="s">
         <v>98</v>
-      </c>
-      <c r="C7" t="s">
-        <v>99</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="60"/>
+      <c r="H7" s="62"/>
       <c r="J7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="14.65" thickBot="1">
@@ -2823,82 +2826,82 @@
         <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H8" s="61"/>
+        <v>28</v>
+      </c>
+      <c r="H8" s="63"/>
       <c r="J8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="H9" s="62"/>
+    </row>
+    <row r="10" spans="1:10" ht="14.65" thickBot="1">
+      <c r="H10" s="63"/>
+      <c r="J10" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
-      <c r="H9" s="60"/>
-    </row>
-    <row r="10" spans="1:10" ht="14.65" thickBot="1">
-      <c r="H10" s="61"/>
-      <c r="J10" t="s">
-        <v>88</v>
-      </c>
-    </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="66"/>
-      <c r="B11" s="62"/>
-      <c r="C11" s="62"/>
-      <c r="D11" s="62"/>
+      <c r="A11" s="60"/>
+      <c r="B11" s="68"/>
+      <c r="C11" s="68"/>
+      <c r="D11" s="68"/>
       <c r="E11" s="70"/>
       <c r="F11" s="70"/>
-      <c r="G11" s="62"/>
-      <c r="H11" s="62"/>
+      <c r="G11" s="68"/>
+      <c r="H11" s="68"/>
       <c r="J11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="14.65" thickBot="1">
-      <c r="A12" s="67"/>
-      <c r="B12" s="63"/>
-      <c r="C12" s="63"/>
-      <c r="D12" s="63"/>
+      <c r="A12" s="61"/>
+      <c r="B12" s="69"/>
+      <c r="C12" s="69"/>
+      <c r="D12" s="69"/>
       <c r="E12" s="71"/>
       <c r="F12" s="71"/>
-      <c r="G12" s="63"/>
-      <c r="H12" s="63"/>
+      <c r="G12" s="69"/>
+      <c r="H12" s="69"/>
       <c r="J12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="J13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="J15" s="58" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="J16" s="59" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="10:10">
       <c r="J17" s="59" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="10:10">
       <c r="J18" s="59" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="10:10">
       <c r="J19" s="59" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2937,7 +2940,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="32.25" customHeight="1" thickBot="1">
       <c r="F1" s="42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G1" s="42"/>
     </row>
@@ -3021,75 +3024,67 @@
       <c r="H7" s="17"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="66"/>
-      <c r="B8" s="60"/>
-      <c r="C8" s="60"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="64"/>
-      <c r="F8" s="64"/>
-      <c r="G8" s="60"/>
-      <c r="H8" s="60"/>
+      <c r="A8" s="60"/>
+      <c r="B8" s="62"/>
+      <c r="C8" s="62"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="66"/>
+      <c r="F8" s="66"/>
+      <c r="G8" s="62"/>
+      <c r="H8" s="62"/>
     </row>
     <row r="9" spans="1:10" ht="14.65" thickBot="1">
-      <c r="A9" s="67"/>
-      <c r="B9" s="61"/>
-      <c r="C9" s="61"/>
-      <c r="D9" s="69"/>
-      <c r="E9" s="65"/>
-      <c r="F9" s="65"/>
-      <c r="G9" s="61"/>
-      <c r="H9" s="61"/>
+      <c r="A9" s="61"/>
+      <c r="B9" s="63"/>
+      <c r="C9" s="63"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="67"/>
+      <c r="G9" s="63"/>
+      <c r="H9" s="63"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="66"/>
-      <c r="B10" s="60"/>
-      <c r="C10" s="60"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="64"/>
-      <c r="F10" s="64"/>
-      <c r="G10" s="60"/>
-      <c r="H10" s="60"/>
+      <c r="A10" s="60"/>
+      <c r="B10" s="62"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="66"/>
+      <c r="F10" s="66"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="62"/>
     </row>
     <row r="11" spans="1:10" ht="14.65" thickBot="1">
-      <c r="A11" s="67"/>
-      <c r="B11" s="61"/>
-      <c r="C11" s="61"/>
-      <c r="D11" s="61"/>
-      <c r="E11" s="65"/>
-      <c r="F11" s="65"/>
-      <c r="G11" s="61"/>
-      <c r="H11" s="61"/>
+      <c r="A11" s="61"/>
+      <c r="B11" s="63"/>
+      <c r="C11" s="63"/>
+      <c r="D11" s="63"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="67"/>
+      <c r="G11" s="63"/>
+      <c r="H11" s="63"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="66"/>
-      <c r="B12" s="62"/>
-      <c r="C12" s="62"/>
-      <c r="D12" s="62"/>
+      <c r="A12" s="60"/>
+      <c r="B12" s="68"/>
+      <c r="C12" s="68"/>
+      <c r="D12" s="68"/>
       <c r="E12" s="70"/>
       <c r="F12" s="70"/>
-      <c r="G12" s="62"/>
-      <c r="H12" s="62"/>
+      <c r="G12" s="68"/>
+      <c r="H12" s="68"/>
     </row>
     <row r="13" spans="1:10" ht="14.65" thickBot="1">
-      <c r="A13" s="67"/>
-      <c r="B13" s="63"/>
-      <c r="C13" s="63"/>
-      <c r="D13" s="63"/>
+      <c r="A13" s="61"/>
+      <c r="B13" s="69"/>
+      <c r="C13" s="69"/>
+      <c r="D13" s="69"/>
       <c r="E13" s="71"/>
       <c r="F13" s="71"/>
-      <c r="G13" s="63"/>
-      <c r="H13" s="63"/>
+      <c r="G13" s="69"/>
+      <c r="H13" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="H8:H9"/>
     <mergeCell ref="A10:A11"/>
@@ -3106,6 +3101,14 @@
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3130,11 +3133,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="39" customHeight="1" thickBot="1">
       <c r="F1" s="42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G1" s="42"/>
       <c r="H1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="23.65" thickBot="1">
@@ -3217,75 +3220,67 @@
       <c r="H7" s="17"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="66"/>
-      <c r="B8" s="60"/>
-      <c r="C8" s="60"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="64"/>
-      <c r="F8" s="64"/>
-      <c r="G8" s="60"/>
-      <c r="H8" s="60"/>
+      <c r="A8" s="60"/>
+      <c r="B8" s="62"/>
+      <c r="C8" s="62"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="66"/>
+      <c r="F8" s="66"/>
+      <c r="G8" s="62"/>
+      <c r="H8" s="62"/>
     </row>
     <row r="9" spans="1:10" ht="14.65" thickBot="1">
-      <c r="A9" s="67"/>
-      <c r="B9" s="61"/>
-      <c r="C9" s="61"/>
-      <c r="D9" s="69"/>
-      <c r="E9" s="65"/>
-      <c r="F9" s="65"/>
-      <c r="G9" s="61"/>
-      <c r="H9" s="61"/>
+      <c r="A9" s="61"/>
+      <c r="B9" s="63"/>
+      <c r="C9" s="63"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="67"/>
+      <c r="G9" s="63"/>
+      <c r="H9" s="63"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="66"/>
-      <c r="B10" s="60"/>
-      <c r="C10" s="60"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="64"/>
-      <c r="F10" s="64"/>
-      <c r="G10" s="60"/>
-      <c r="H10" s="60"/>
+      <c r="A10" s="60"/>
+      <c r="B10" s="62"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="66"/>
+      <c r="F10" s="66"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="62"/>
     </row>
     <row r="11" spans="1:10" ht="14.65" thickBot="1">
-      <c r="A11" s="67"/>
-      <c r="B11" s="61"/>
-      <c r="C11" s="61"/>
-      <c r="D11" s="61"/>
-      <c r="E11" s="65"/>
-      <c r="F11" s="65"/>
-      <c r="G11" s="61"/>
-      <c r="H11" s="61"/>
+      <c r="A11" s="61"/>
+      <c r="B11" s="63"/>
+      <c r="C11" s="63"/>
+      <c r="D11" s="63"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="67"/>
+      <c r="G11" s="63"/>
+      <c r="H11" s="63"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="66"/>
-      <c r="B12" s="62"/>
-      <c r="C12" s="62"/>
-      <c r="D12" s="62"/>
+      <c r="A12" s="60"/>
+      <c r="B12" s="68"/>
+      <c r="C12" s="68"/>
+      <c r="D12" s="68"/>
       <c r="E12" s="70"/>
       <c r="F12" s="70"/>
-      <c r="G12" s="62"/>
-      <c r="H12" s="62"/>
+      <c r="G12" s="68"/>
+      <c r="H12" s="68"/>
     </row>
     <row r="13" spans="1:10" ht="14.65" thickBot="1">
-      <c r="A13" s="67"/>
-      <c r="B13" s="63"/>
-      <c r="C13" s="63"/>
-      <c r="D13" s="63"/>
+      <c r="A13" s="61"/>
+      <c r="B13" s="69"/>
+      <c r="C13" s="69"/>
+      <c r="D13" s="69"/>
       <c r="E13" s="71"/>
       <c r="F13" s="71"/>
-      <c r="G13" s="63"/>
-      <c r="H13" s="63"/>
+      <c r="G13" s="69"/>
+      <c r="H13" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="H8:H9"/>
     <mergeCell ref="A10:A11"/>
@@ -3302,6 +3297,14 @@
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3405,75 +3408,67 @@
       <c r="H7" s="17"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="66"/>
-      <c r="B8" s="60"/>
-      <c r="C8" s="60"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="64"/>
-      <c r="F8" s="64"/>
-      <c r="G8" s="60"/>
-      <c r="H8" s="60"/>
+      <c r="A8" s="60"/>
+      <c r="B8" s="62"/>
+      <c r="C8" s="62"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="66"/>
+      <c r="F8" s="66"/>
+      <c r="G8" s="62"/>
+      <c r="H8" s="62"/>
     </row>
     <row r="9" spans="1:10" ht="14.65" thickBot="1">
-      <c r="A9" s="67"/>
-      <c r="B9" s="61"/>
-      <c r="C9" s="61"/>
-      <c r="D9" s="69"/>
-      <c r="E9" s="65"/>
-      <c r="F9" s="65"/>
-      <c r="G9" s="61"/>
-      <c r="H9" s="61"/>
+      <c r="A9" s="61"/>
+      <c r="B9" s="63"/>
+      <c r="C9" s="63"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="67"/>
+      <c r="G9" s="63"/>
+      <c r="H9" s="63"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="66"/>
-      <c r="B10" s="60"/>
-      <c r="C10" s="60"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="64"/>
-      <c r="F10" s="64"/>
-      <c r="G10" s="60"/>
-      <c r="H10" s="60"/>
+      <c r="A10" s="60"/>
+      <c r="B10" s="62"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="66"/>
+      <c r="F10" s="66"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="62"/>
     </row>
     <row r="11" spans="1:10" ht="14.65" thickBot="1">
-      <c r="A11" s="67"/>
-      <c r="B11" s="61"/>
-      <c r="C11" s="61"/>
-      <c r="D11" s="61"/>
-      <c r="E11" s="65"/>
-      <c r="F11" s="65"/>
-      <c r="G11" s="61"/>
-      <c r="H11" s="61"/>
+      <c r="A11" s="61"/>
+      <c r="B11" s="63"/>
+      <c r="C11" s="63"/>
+      <c r="D11" s="63"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="67"/>
+      <c r="G11" s="63"/>
+      <c r="H11" s="63"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="66"/>
-      <c r="B12" s="62"/>
-      <c r="C12" s="62"/>
-      <c r="D12" s="62"/>
+      <c r="A12" s="60"/>
+      <c r="B12" s="68"/>
+      <c r="C12" s="68"/>
+      <c r="D12" s="68"/>
       <c r="E12" s="70"/>
       <c r="F12" s="70"/>
-      <c r="G12" s="62"/>
-      <c r="H12" s="62"/>
+      <c r="G12" s="68"/>
+      <c r="H12" s="68"/>
     </row>
     <row r="13" spans="1:10" ht="14.65" thickBot="1">
-      <c r="A13" s="67"/>
-      <c r="B13" s="63"/>
-      <c r="C13" s="63"/>
-      <c r="D13" s="63"/>
+      <c r="A13" s="61"/>
+      <c r="B13" s="69"/>
+      <c r="C13" s="69"/>
+      <c r="D13" s="69"/>
       <c r="E13" s="71"/>
       <c r="F13" s="71"/>
-      <c r="G13" s="63"/>
-      <c r="H13" s="63"/>
+      <c r="G13" s="69"/>
+      <c r="H13" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="H8:H9"/>
     <mergeCell ref="A10:A11"/>
@@ -3490,6 +3485,14 @@
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3510,7 +3513,7 @@
   <sheetData>
     <row r="2" spans="1:2">
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -3518,7 +3521,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -3526,7 +3529,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2">

</xml_diff>

<commit_message>
added changes to the domain model
</commit_message>
<xml_diff>
--- a/bea-documentation/sprint-backlog/sprint-backlog.xlsx
+++ b/bea-documentation/sprint-backlog/sprint-backlog.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6233DACC-E7C1-423A-B215-FDCDED8FB2AC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{352787F0-BE6F-420F-BB2A-0B3A477C30AD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sprint plan" sheetId="8" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="100">
   <si>
     <t>Estimated Effort</t>
   </si>
@@ -179,18 +179,6 @@
   </si>
   <si>
     <t>Meetings time 14:30- 15:00</t>
-  </si>
-  <si>
-    <t>del 1</t>
-  </si>
-  <si>
-    <t>del2</t>
-  </si>
-  <si>
-    <t>del3</t>
-  </si>
-  <si>
-    <t>del4</t>
   </si>
   <si>
     <t>Goals</t>
@@ -350,7 +338,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -396,6 +384,13 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="2"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -713,7 +708,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -797,9 +792,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
@@ -822,22 +814,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -846,10 +832,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -857,6 +849,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1654,8 +1652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52C5C85A-82B4-4FC3-85DE-ADD80C9606CE}">
   <dimension ref="A1:AC22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X9" sqref="X9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1981,22 +1979,22 @@
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="23"/>
-      <c r="H7" s="43">
+      <c r="H7" s="42">
         <v>2</v>
       </c>
-      <c r="I7" s="43"/>
-      <c r="J7" s="43"/>
-      <c r="K7" s="44">
+      <c r="I7" s="42"/>
+      <c r="J7" s="42"/>
+      <c r="K7" s="43"/>
+      <c r="L7" s="43">
         <v>3</v>
       </c>
-      <c r="L7" s="44"/>
-      <c r="M7" s="44"/>
-      <c r="N7" s="45">
+      <c r="M7" s="43"/>
+      <c r="N7" s="44">
         <v>4</v>
       </c>
-      <c r="O7" s="45"/>
-      <c r="P7" s="45"/>
-      <c r="Q7" s="45"/>
+      <c r="O7" s="44"/>
+      <c r="P7" s="44"/>
+      <c r="Q7" s="44"/>
       <c r="R7" s="22"/>
       <c r="S7" s="22"/>
       <c r="T7" s="25"/>
@@ -2019,25 +2017,17 @@
       <c r="D8" s="22"/>
       <c r="E8" s="22"/>
       <c r="F8" s="22"/>
-      <c r="G8" s="22" t="s">
-        <v>49</v>
-      </c>
+      <c r="G8" s="22"/>
       <c r="H8" s="22"/>
       <c r="I8" s="22"/>
-      <c r="J8" s="22" t="s">
-        <v>50</v>
-      </c>
+      <c r="J8" s="22"/>
       <c r="K8" s="22"/>
       <c r="L8" s="22"/>
-      <c r="M8" s="22" t="s">
-        <v>51</v>
-      </c>
+      <c r="M8" s="22"/>
       <c r="N8" s="22"/>
       <c r="O8" s="22"/>
       <c r="P8" s="22"/>
-      <c r="Q8" s="22" t="s">
-        <v>52</v>
-      </c>
+      <c r="Q8" s="22"/>
       <c r="R8" s="22"/>
       <c r="S8" s="22"/>
       <c r="T8" s="25"/>
@@ -2156,7 +2146,7 @@
       <c r="U12" s="33"/>
       <c r="V12" s="30"/>
       <c r="W12" s="30"/>
-      <c r="X12" s="35">
+      <c r="X12" s="71">
         <v>6</v>
       </c>
       <c r="Y12" s="30"/>
@@ -2169,7 +2159,7 @@
       <c r="U13" s="33"/>
       <c r="V13" s="30"/>
       <c r="W13" s="30"/>
-      <c r="X13" s="35">
+      <c r="X13" s="71">
         <v>13</v>
       </c>
       <c r="Y13" s="30"/>
@@ -2183,7 +2173,7 @@
       <c r="U14" s="33"/>
       <c r="V14" s="30"/>
       <c r="W14" s="30"/>
-      <c r="X14" s="35">
+      <c r="X14" s="71">
         <v>20</v>
       </c>
       <c r="Y14" s="30"/>
@@ -2197,7 +2187,7 @@
       <c r="U15" s="33"/>
       <c r="V15" s="30"/>
       <c r="W15" s="30"/>
-      <c r="X15" s="35">
+      <c r="X15" s="71">
         <v>27</v>
       </c>
       <c r="Y15" s="30"/>
@@ -2213,7 +2203,7 @@
         <v>43800</v>
       </c>
       <c r="W16" s="30"/>
-      <c r="X16" s="35"/>
+      <c r="X16" s="71"/>
       <c r="Y16" s="30"/>
       <c r="Z16" s="30"/>
       <c r="AA16" s="30"/>
@@ -2225,7 +2215,7 @@
       <c r="U17" s="33"/>
       <c r="V17" s="30"/>
       <c r="W17" s="30"/>
-      <c r="X17" s="35">
+      <c r="X17" s="71">
         <v>4</v>
       </c>
       <c r="Y17" s="30"/>
@@ -2239,7 +2229,7 @@
       <c r="U18" s="33"/>
       <c r="V18" s="30"/>
       <c r="W18" s="30"/>
-      <c r="X18" s="35">
+      <c r="X18" s="71">
         <v>11</v>
       </c>
       <c r="Y18" s="30"/>
@@ -2252,14 +2242,14 @@
       <c r="U19" s="37"/>
       <c r="V19" s="38"/>
       <c r="W19" s="38"/>
-      <c r="X19" s="39">
+      <c r="X19" s="72">
         <v>18</v>
       </c>
       <c r="Y19" s="38"/>
       <c r="Z19" s="38"/>
       <c r="AA19" s="38"/>
       <c r="AB19" s="38"/>
-      <c r="AC19" s="40"/>
+      <c r="AC19" s="39"/>
     </row>
     <row r="20" spans="4:29">
       <c r="V20" s="25"/>
@@ -2280,12 +2270,12 @@
       <c r="AB21" s="25"/>
     </row>
     <row r="22" spans="4:29">
-      <c r="V22" s="41" t="s">
+      <c r="V22" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="W22" s="41"/>
-      <c r="X22" s="41"/>
-      <c r="Y22" s="41"/>
+      <c r="W22" s="40"/>
+      <c r="X22" s="40"/>
+      <c r="Y22" s="40"/>
       <c r="Z22" s="25"/>
       <c r="AA22" s="25"/>
       <c r="AB22" s="25"/>
@@ -2300,7 +2290,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -2319,13 +2309,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="32.25" customHeight="1" thickBot="1">
-      <c r="C1" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="F1" s="42" t="s">
-        <v>77</v>
-      </c>
-      <c r="G1" s="42"/>
+      <c r="C1" s="47" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" s="41" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" s="41"/>
     </row>
     <row r="2" spans="1:10" ht="58.5" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -2350,11 +2340,11 @@
         <v>2</v>
       </c>
       <c r="H2" s="3"/>
-      <c r="I2" s="51" t="s">
-        <v>53</v>
-      </c>
-      <c r="J2" s="52" t="s">
-        <v>58</v>
+      <c r="I2" s="50" t="s">
+        <v>49</v>
+      </c>
+      <c r="J2" s="51" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="14.65" thickBot="1">
@@ -2376,11 +2366,11 @@
         <v>18</v>
       </c>
       <c r="H3" s="6"/>
-      <c r="I3" s="53" t="s">
-        <v>54</v>
-      </c>
-      <c r="J3" s="54" t="s">
-        <v>60</v>
+      <c r="I3" s="52" t="s">
+        <v>50</v>
+      </c>
+      <c r="J3" s="53" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="23.25">
@@ -2402,11 +2392,11 @@
         <v>18</v>
       </c>
       <c r="H4" s="19"/>
-      <c r="I4" s="55" t="s">
+      <c r="I4" s="54" t="s">
+        <v>51</v>
+      </c>
+      <c r="J4" s="55" t="s">
         <v>55</v>
-      </c>
-      <c r="J4" s="56" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="14.65" thickBot="1">
@@ -2428,11 +2418,11 @@
         <v>18</v>
       </c>
       <c r="H5" s="20"/>
-      <c r="I5" s="53" t="s">
+      <c r="I5" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="54" t="s">
-        <v>64</v>
+      <c r="J5" s="53" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="14.65" thickBot="1">
@@ -2454,11 +2444,11 @@
         <v>18</v>
       </c>
       <c r="H6" s="21"/>
-      <c r="I6" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="J6" s="56" t="s">
-        <v>61</v>
+      <c r="I6" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="J6" s="55" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="14.65" thickBot="1">
@@ -2481,12 +2471,12 @@
       <c r="G7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="62"/>
-      <c r="I7" s="53" t="s">
-        <v>57</v>
-      </c>
-      <c r="J7" s="54" t="s">
-        <v>62</v>
+      <c r="H7" s="59"/>
+      <c r="I7" s="52" t="s">
+        <v>53</v>
+      </c>
+      <c r="J7" s="53" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="14.65" thickBot="1">
@@ -2507,12 +2497,12 @@
       <c r="G8" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="63"/>
-      <c r="I8" s="55" t="s">
-        <v>101</v>
-      </c>
-      <c r="J8" s="56" t="s">
-        <v>63</v>
+      <c r="H8" s="60"/>
+      <c r="I8" s="54" t="s">
+        <v>97</v>
+      </c>
+      <c r="J8" s="55" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="14.65" thickBot="1">
@@ -2533,12 +2523,12 @@
       <c r="G9" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="H9" s="62"/>
-      <c r="I9" s="53" t="s">
-        <v>102</v>
-      </c>
-      <c r="J9" s="54" t="s">
-        <v>65</v>
+      <c r="H9" s="59"/>
+      <c r="I9" s="52" t="s">
+        <v>98</v>
+      </c>
+      <c r="J9" s="53" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="23.65" thickBot="1">
@@ -2557,12 +2547,12 @@
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
       <c r="G10" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="H10" s="63"/>
-      <c r="I10" s="55"/>
-      <c r="J10" s="56" t="s">
-        <v>66</v>
+        <v>96</v>
+      </c>
+      <c r="H10" s="60"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="55" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="23.65" thickBot="1">
@@ -2573,93 +2563,85 @@
         <v>25</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
       <c r="G11" s="17"/>
-      <c r="H11" s="68"/>
-      <c r="I11" s="53"/>
-      <c r="J11" s="54"/>
+      <c r="H11" s="61"/>
+      <c r="I11" s="52"/>
+      <c r="J11" s="53"/>
     </row>
     <row r="12" spans="1:10" ht="14.65" thickBot="1">
-      <c r="A12" s="60">
+      <c r="A12" s="65">
         <v>10</v>
       </c>
-      <c r="B12" s="68" t="s">
+      <c r="B12" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="68" t="s">
+      <c r="C12" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="68" t="s">
+      <c r="D12" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="66"/>
-      <c r="F12" s="66"/>
-      <c r="G12" s="62" t="s">
+      <c r="E12" s="63"/>
+      <c r="F12" s="63"/>
+      <c r="G12" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="69"/>
-      <c r="I12" s="55"/>
-      <c r="J12" s="56"/>
+      <c r="H12" s="62"/>
+      <c r="I12" s="54"/>
+      <c r="J12" s="55"/>
     </row>
     <row r="13" spans="1:10" ht="14.65" thickBot="1">
-      <c r="A13" s="61"/>
-      <c r="B13" s="69"/>
-      <c r="C13" s="69"/>
-      <c r="D13" s="69"/>
-      <c r="E13" s="67"/>
-      <c r="F13" s="67"/>
-      <c r="G13" s="63"/>
-      <c r="I13" s="53"/>
-      <c r="J13" s="54"/>
+      <c r="A13" s="66"/>
+      <c r="B13" s="62"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="64"/>
+      <c r="F13" s="64"/>
+      <c r="G13" s="60"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="53"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="60">
+      <c r="A14" s="65">
         <v>11</v>
       </c>
-      <c r="B14" s="62" t="s">
+      <c r="B14" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="62" t="s">
-        <v>103</v>
-      </c>
-      <c r="D14" s="64" t="s">
+      <c r="C14" s="59" t="s">
+        <v>99</v>
+      </c>
+      <c r="D14" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="66"/>
-      <c r="F14" s="66"/>
-      <c r="G14" s="62" t="s">
+      <c r="E14" s="63"/>
+      <c r="F14" s="63"/>
+      <c r="G14" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="I14" s="49"/>
-      <c r="J14" s="50"/>
+      <c r="I14" s="48"/>
+      <c r="J14" s="49"/>
     </row>
     <row r="15" spans="1:10" ht="14.65" thickBot="1">
-      <c r="A15" s="61"/>
-      <c r="B15" s="63"/>
-      <c r="C15" s="63"/>
-      <c r="D15" s="65"/>
-      <c r="E15" s="67"/>
-      <c r="F15" s="67"/>
-      <c r="G15" s="63"/>
+      <c r="A15" s="66"/>
+      <c r="B15" s="60"/>
+      <c r="C15" s="60"/>
+      <c r="D15" s="68"/>
+      <c r="E15" s="64"/>
+      <c r="F15" s="64"/>
+      <c r="G15" s="60"/>
     </row>
     <row r="18" spans="3:3" ht="23.25" customHeight="1"/>
     <row r="30" spans="3:3">
-      <c r="C30" s="47"/>
+      <c r="C30" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="F12:F13"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="C14:C15"/>
@@ -2669,6 +2651,14 @@
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="F12:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2679,7 +2669,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="A3" sqref="A3:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2693,13 +2683,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="34.5" customHeight="1" thickBot="1">
-      <c r="C1" s="47" t="s">
-        <v>68</v>
-      </c>
-      <c r="F1" s="42" t="s">
-        <v>78</v>
-      </c>
-      <c r="G1" s="42"/>
+      <c r="C1" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" s="41" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" s="41"/>
     </row>
     <row r="2" spans="1:10" ht="23.65" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -2724,11 +2714,11 @@
         <v>2</v>
       </c>
       <c r="H2" s="3"/>
-      <c r="I2" s="46" t="s">
-        <v>53</v>
-      </c>
-      <c r="J2" s="57" t="s">
-        <v>58</v>
+      <c r="I2" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="J2" s="56" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="26.65" customHeight="1">
@@ -2736,17 +2726,17 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
       </c>
       <c r="H3" s="10"/>
       <c r="J3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="20.25" customHeight="1" thickBot="1">
@@ -2754,17 +2744,17 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
       </c>
       <c r="H4" s="13"/>
       <c r="J4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="18" customHeight="1">
@@ -2772,17 +2762,17 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
       </c>
       <c r="H5" s="16"/>
       <c r="J5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="18.75" customHeight="1" thickBot="1">
@@ -2790,10 +2780,10 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
@@ -2808,17 +2798,17 @@
         <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="62"/>
+      <c r="H7" s="59"/>
       <c r="J7" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="14.65" thickBot="1">
@@ -2826,82 +2816,82 @@
         <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C8" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D8" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="63"/>
+      <c r="H8" s="60"/>
       <c r="J8" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="H9" s="62"/>
+      <c r="H9" s="59"/>
     </row>
     <row r="10" spans="1:10" ht="14.65" thickBot="1">
-      <c r="H10" s="63"/>
+      <c r="H10" s="60"/>
       <c r="J10" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="60"/>
-      <c r="B11" s="68"/>
-      <c r="C11" s="68"/>
-      <c r="D11" s="68"/>
-      <c r="E11" s="70"/>
-      <c r="F11" s="70"/>
-      <c r="G11" s="68"/>
-      <c r="H11" s="68"/>
+      <c r="A11" s="65"/>
+      <c r="B11" s="61"/>
+      <c r="C11" s="61"/>
+      <c r="D11" s="61"/>
+      <c r="E11" s="69"/>
+      <c r="F11" s="69"/>
+      <c r="G11" s="61"/>
+      <c r="H11" s="61"/>
       <c r="J11" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="14.65" thickBot="1">
-      <c r="A12" s="61"/>
-      <c r="B12" s="69"/>
-      <c r="C12" s="69"/>
-      <c r="D12" s="69"/>
-      <c r="E12" s="71"/>
-      <c r="F12" s="71"/>
-      <c r="G12" s="69"/>
-      <c r="H12" s="69"/>
+      <c r="A12" s="66"/>
+      <c r="B12" s="62"/>
+      <c r="C12" s="62"/>
+      <c r="D12" s="62"/>
+      <c r="E12" s="70"/>
+      <c r="F12" s="70"/>
+      <c r="G12" s="62"/>
+      <c r="H12" s="62"/>
       <c r="J12" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="J13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="J15" s="57" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="J16" s="58" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="10:10">
+      <c r="J17" s="58" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="10:10">
+      <c r="J18" s="58" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
-      <c r="J15" s="58" t="s">
+    <row r="19" spans="10:10">
+      <c r="J19" s="58" t="s">
         <v>90</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="J16" s="59" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="17" spans="10:10">
-      <c r="J17" s="59" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="18" spans="10:10">
-      <c r="J18" s="59" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="19" spans="10:10">
-      <c r="J19" s="59" t="s">
-        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2939,10 +2929,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="32.25" customHeight="1" thickBot="1">
-      <c r="F1" s="42" t="s">
-        <v>79</v>
-      </c>
-      <c r="G1" s="42"/>
+      <c r="F1" s="41" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" s="41"/>
     </row>
     <row r="2" spans="1:10" ht="23.65" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -3024,67 +3014,75 @@
       <c r="H7" s="17"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="60"/>
-      <c r="B8" s="62"/>
-      <c r="C8" s="62"/>
-      <c r="D8" s="64"/>
-      <c r="E8" s="66"/>
-      <c r="F8" s="66"/>
-      <c r="G8" s="62"/>
-      <c r="H8" s="62"/>
+      <c r="A8" s="65"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="63"/>
+      <c r="G8" s="59"/>
+      <c r="H8" s="59"/>
     </row>
     <row r="9" spans="1:10" ht="14.65" thickBot="1">
-      <c r="A9" s="61"/>
-      <c r="B9" s="63"/>
-      <c r="C9" s="63"/>
-      <c r="D9" s="65"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="67"/>
-      <c r="G9" s="63"/>
-      <c r="H9" s="63"/>
+      <c r="A9" s="66"/>
+      <c r="B9" s="60"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="60"/>
+      <c r="H9" s="60"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="60"/>
-      <c r="B10" s="62"/>
-      <c r="C10" s="62"/>
-      <c r="D10" s="62"/>
-      <c r="E10" s="66"/>
-      <c r="F10" s="66"/>
-      <c r="G10" s="62"/>
-      <c r="H10" s="62"/>
+      <c r="A10" s="65"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="63"/>
+      <c r="G10" s="59"/>
+      <c r="H10" s="59"/>
     </row>
     <row r="11" spans="1:10" ht="14.65" thickBot="1">
-      <c r="A11" s="61"/>
-      <c r="B11" s="63"/>
-      <c r="C11" s="63"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="67"/>
-      <c r="F11" s="67"/>
-      <c r="G11" s="63"/>
-      <c r="H11" s="63"/>
+      <c r="A11" s="66"/>
+      <c r="B11" s="60"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="60"/>
+      <c r="H11" s="60"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="60"/>
-      <c r="B12" s="68"/>
-      <c r="C12" s="68"/>
-      <c r="D12" s="68"/>
-      <c r="E12" s="70"/>
-      <c r="F12" s="70"/>
-      <c r="G12" s="68"/>
-      <c r="H12" s="68"/>
+      <c r="A12" s="65"/>
+      <c r="B12" s="61"/>
+      <c r="C12" s="61"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="69"/>
+      <c r="G12" s="61"/>
+      <c r="H12" s="61"/>
     </row>
     <row r="13" spans="1:10" ht="14.65" thickBot="1">
-      <c r="A13" s="61"/>
-      <c r="B13" s="69"/>
-      <c r="C13" s="69"/>
-      <c r="D13" s="69"/>
-      <c r="E13" s="71"/>
-      <c r="F13" s="71"/>
-      <c r="G13" s="69"/>
-      <c r="H13" s="69"/>
+      <c r="A13" s="66"/>
+      <c r="B13" s="62"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="70"/>
+      <c r="F13" s="70"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="H8:H9"/>
     <mergeCell ref="A10:A11"/>
@@ -3101,14 +3099,6 @@
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3132,12 +3122,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="39" customHeight="1" thickBot="1">
-      <c r="F1" s="42" t="s">
-        <v>80</v>
-      </c>
-      <c r="G1" s="42"/>
+      <c r="F1" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" s="41"/>
       <c r="H1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="23.65" thickBot="1">
@@ -3220,67 +3210,75 @@
       <c r="H7" s="17"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="60"/>
-      <c r="B8" s="62"/>
-      <c r="C8" s="62"/>
-      <c r="D8" s="64"/>
-      <c r="E8" s="66"/>
-      <c r="F8" s="66"/>
-      <c r="G8" s="62"/>
-      <c r="H8" s="62"/>
+      <c r="A8" s="65"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="63"/>
+      <c r="G8" s="59"/>
+      <c r="H8" s="59"/>
     </row>
     <row r="9" spans="1:10" ht="14.65" thickBot="1">
-      <c r="A9" s="61"/>
-      <c r="B9" s="63"/>
-      <c r="C9" s="63"/>
-      <c r="D9" s="65"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="67"/>
-      <c r="G9" s="63"/>
-      <c r="H9" s="63"/>
+      <c r="A9" s="66"/>
+      <c r="B9" s="60"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="60"/>
+      <c r="H9" s="60"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="60"/>
-      <c r="B10" s="62"/>
-      <c r="C10" s="62"/>
-      <c r="D10" s="62"/>
-      <c r="E10" s="66"/>
-      <c r="F10" s="66"/>
-      <c r="G10" s="62"/>
-      <c r="H10" s="62"/>
+      <c r="A10" s="65"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="63"/>
+      <c r="G10" s="59"/>
+      <c r="H10" s="59"/>
     </row>
     <row r="11" spans="1:10" ht="14.65" thickBot="1">
-      <c r="A11" s="61"/>
-      <c r="B11" s="63"/>
-      <c r="C11" s="63"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="67"/>
-      <c r="F11" s="67"/>
-      <c r="G11" s="63"/>
-      <c r="H11" s="63"/>
+      <c r="A11" s="66"/>
+      <c r="B11" s="60"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="60"/>
+      <c r="H11" s="60"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="60"/>
-      <c r="B12" s="68"/>
-      <c r="C12" s="68"/>
-      <c r="D12" s="68"/>
-      <c r="E12" s="70"/>
-      <c r="F12" s="70"/>
-      <c r="G12" s="68"/>
-      <c r="H12" s="68"/>
+      <c r="A12" s="65"/>
+      <c r="B12" s="61"/>
+      <c r="C12" s="61"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="69"/>
+      <c r="G12" s="61"/>
+      <c r="H12" s="61"/>
     </row>
     <row r="13" spans="1:10" ht="14.65" thickBot="1">
-      <c r="A13" s="61"/>
-      <c r="B13" s="69"/>
-      <c r="C13" s="69"/>
-      <c r="D13" s="69"/>
-      <c r="E13" s="71"/>
-      <c r="F13" s="71"/>
-      <c r="G13" s="69"/>
-      <c r="H13" s="69"/>
+      <c r="A13" s="66"/>
+      <c r="B13" s="62"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="70"/>
+      <c r="F13" s="70"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="H8:H9"/>
     <mergeCell ref="A10:A11"/>
@@ -3297,14 +3295,6 @@
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3408,67 +3398,75 @@
       <c r="H7" s="17"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="60"/>
-      <c r="B8" s="62"/>
-      <c r="C8" s="62"/>
-      <c r="D8" s="64"/>
-      <c r="E8" s="66"/>
-      <c r="F8" s="66"/>
-      <c r="G8" s="62"/>
-      <c r="H8" s="62"/>
+      <c r="A8" s="65"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="63"/>
+      <c r="G8" s="59"/>
+      <c r="H8" s="59"/>
     </row>
     <row r="9" spans="1:10" ht="14.65" thickBot="1">
-      <c r="A9" s="61"/>
-      <c r="B9" s="63"/>
-      <c r="C9" s="63"/>
-      <c r="D9" s="65"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="67"/>
-      <c r="G9" s="63"/>
-      <c r="H9" s="63"/>
+      <c r="A9" s="66"/>
+      <c r="B9" s="60"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="60"/>
+      <c r="H9" s="60"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="60"/>
-      <c r="B10" s="62"/>
-      <c r="C10" s="62"/>
-      <c r="D10" s="62"/>
-      <c r="E10" s="66"/>
-      <c r="F10" s="66"/>
-      <c r="G10" s="62"/>
-      <c r="H10" s="62"/>
+      <c r="A10" s="65"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="63"/>
+      <c r="G10" s="59"/>
+      <c r="H10" s="59"/>
     </row>
     <row r="11" spans="1:10" ht="14.65" thickBot="1">
-      <c r="A11" s="61"/>
-      <c r="B11" s="63"/>
-      <c r="C11" s="63"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="67"/>
-      <c r="F11" s="67"/>
-      <c r="G11" s="63"/>
-      <c r="H11" s="63"/>
+      <c r="A11" s="66"/>
+      <c r="B11" s="60"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="60"/>
+      <c r="H11" s="60"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="60"/>
-      <c r="B12" s="68"/>
-      <c r="C12" s="68"/>
-      <c r="D12" s="68"/>
-      <c r="E12" s="70"/>
-      <c r="F12" s="70"/>
-      <c r="G12" s="68"/>
-      <c r="H12" s="68"/>
+      <c r="A12" s="65"/>
+      <c r="B12" s="61"/>
+      <c r="C12" s="61"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="69"/>
+      <c r="G12" s="61"/>
+      <c r="H12" s="61"/>
     </row>
     <row r="13" spans="1:10" ht="14.65" thickBot="1">
-      <c r="A13" s="61"/>
-      <c r="B13" s="69"/>
-      <c r="C13" s="69"/>
-      <c r="D13" s="69"/>
-      <c r="E13" s="71"/>
-      <c r="F13" s="71"/>
-      <c r="G13" s="69"/>
-      <c r="H13" s="69"/>
+      <c r="A13" s="66"/>
+      <c r="B13" s="62"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="70"/>
+      <c r="F13" s="70"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="H8:H9"/>
     <mergeCell ref="A10:A11"/>
@@ -3485,14 +3483,6 @@
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>